<commit_message>
Results in 920 revamped
</commit_message>
<xml_diff>
--- a/strategies/Results/Back_Testing_Results_Sample.xlsx
+++ b/strategies/Results/Back_Testing_Results_Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Abhishek_Koshta\Personal\Investment\Back Testing\market-analysis\Zerodha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Abhishek_Koshta\Personal\Investment\Back Testing\market-analysis\strategies\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C332F127-1E98-42D4-AE08-9254F1C4B919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A3059-EA8D-474F-856A-BF5E1E64C186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Total signals generated</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>Max losing streak</t>
+  </si>
+  <si>
+    <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t>Reverse Entry</t>
+  </si>
+  <si>
+    <t>Reverse_Exit</t>
+  </si>
+  <si>
+    <t>R_Close_Exit</t>
+  </si>
+  <si>
+    <t>R_Close_Entry</t>
   </si>
 </sst>
 </file>
@@ -473,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,15 +680,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B5B1FA-8E6D-4348-BA19-04C761F1ED5F}">
-  <dimension ref="B1:E1"/>
+  <dimension ref="B1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>28</v>
       </c>
@@ -685,6 +705,21 @@
       </c>
       <c r="E1" t="s">
         <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>